<commit_message>
Basic stuff works, old code removed
</commit_message>
<xml_diff>
--- a/xplmod/excel.mod/test/test-modify.xlsx
+++ b/xplmod/excel.mod/test/test-modify.xlsx
@@ -1,91 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Erik\work\xatapult\xtpxlib-xoffice\xplmod\excel.mod\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0157D796-40A0-4C8C-B057-A156D67FBE64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="84" windowWidth="22848" windowHeight="9360"/>
+    <workbookView xWindow="2200" yWindow="2200" windowWidth="18300" windowHeight="10520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEST" sheetId="3" r:id="rId1"/>
-    <sheet name="Eerste werkblad" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" refMode="R1C1"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Erik Siegel</author>
-  </authors>
-  <commentList>
-    <comment ref="C4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Erik Siegel:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Opmerking!</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Totaal</t>
-  </si>
-  <si>
-    <t>Rij 5 data</t>
-  </si>
-  <si>
-    <t>En hier nog wat</t>
-  </si>
-  <si>
-    <t>HIERO</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
+    <t>bloebblub</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,23 +49,10 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,17 +72,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
-    <cellStyle name="Valuta" xfId="1" builtinId="4"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -149,14 +88,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -194,9 +136,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,9 +171,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -264,9 +223,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -439,118 +415,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A5:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="1" max="1" width="18.52734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <f>SUM(A2:C2)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1">
-        <f>SUM(A3:C3)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <f>SUM(A4:C4)</f>
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Named cells working (stil contains debug code)
</commit_message>
<xml_diff>
--- a/xplmod/excel.mod/test/test-modify.xlsx
+++ b/xplmod/excel.mod/test/test-modify.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Erik\work\xatapult\xtpxlib-xoffice\xplmod\excel.mod\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0157D796-40A0-4C8C-B057-A156D67FBE64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA9AA09-9822-495D-A35C-AE19AA004283}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="2200" windowWidth="18300" windowHeight="10520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEST" sheetId="3" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="NAMEDCELL">TEST!$E$1</definedName>
+    <definedName name="xx">TEST!$D$1</definedName>
+  </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,9 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>bloebblub</t>
+  </si>
+  <si>
+    <t>HERE</t>
+  </si>
+  <si>
+    <t>Named cell:</t>
   </si>
 </sst>
 </file>
@@ -416,18 +426,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="18.52734375" customWidth="1"/>
+    <col min="4" max="4" width="12.52734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>